<commit_message>
attempting some text cleaning
</commit_message>
<xml_diff>
--- a/telegram_corpus.xlsx
+++ b/telegram_corpus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c315e0645f3ee56d/Data gov 50/Final project/gov50-final/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="235" documentId="8_{6E2AAD70-F8D2-44E6-9A27-31C793069EE0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{DDBADBBD-33A2-47B2-960A-A6691DC281AE}"/>
+  <xr:revisionPtr revIDLastSave="263" documentId="8_{6E2AAD70-F8D2-44E6-9A27-31C793069EE0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D86A6682-A29A-4854-BB0E-440DDE9CA94E}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E642C494-3A5F-4C64-B3BD-CD15303C2502}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="68">
   <si>
     <t>Name</t>
   </si>
@@ -180,9 +180,6 @@
     <t>tribuna_by</t>
   </si>
   <si>
-    <t>studenty_by</t>
-  </si>
-  <si>
     <t>pressmvd</t>
   </si>
   <si>
@@ -226,6 +223,21 @@
   </si>
   <si>
     <t>stop_gaiduk</t>
+  </si>
+  <si>
+    <t>language</t>
+  </si>
+  <si>
+    <t>Russian</t>
+  </si>
+  <si>
+    <t>Belarussian</t>
+  </si>
+  <si>
+    <t>Both</t>
+  </si>
+  <si>
+    <t>studentyBY</t>
   </si>
 </sst>
 </file>
@@ -603,10 +615,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B79CD0CB-8193-4741-A468-87913EFFCABE}">
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -616,7 +628,7 @@
     <col min="3" max="3" width="20.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -624,7 +636,7 @@
         <v>17</v>
       </c>
       <c r="C1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D1" t="s">
         <v>36</v>
@@ -632,8 +644,11 @@
       <c r="E1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -649,8 +664,11 @@
       <c r="E2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -666,8 +684,11 @@
       <c r="E3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
@@ -683,8 +704,11 @@
       <c r="E4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
@@ -700,8 +724,11 @@
       <c r="E5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
@@ -717,8 +744,11 @@
       <c r="E6" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
@@ -734,8 +764,11 @@
       <c r="E7" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
@@ -751,8 +784,11 @@
       <c r="E8" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>8</v>
       </c>
@@ -768,8 +804,11 @@
       <c r="E9" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>9</v>
       </c>
@@ -785,8 +824,11 @@
       <c r="E10" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F10" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -802,8 +844,11 @@
       <c r="E11" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F11" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -819,8 +864,11 @@
       <c r="E12" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F12" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>12</v>
       </c>
@@ -836,8 +884,11 @@
       <c r="E13" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F13" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
         <v>13</v>
       </c>
@@ -853,8 +904,11 @@
       <c r="E14" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F14" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -870,20 +924,23 @@
       <c r="E15" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F15" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
         <v>15</v>
       </c>
       <c r="B16" s="1"/>
       <c r="D16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E16" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
@@ -899,13 +956,16 @@
       <c r="E17" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F17" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C18">
         <v>1338</v>
@@ -916,13 +976,16 @@
       <c r="E18" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F18" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C19">
         <v>1581</v>
@@ -933,13 +996,16 @@
       <c r="E19" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F19" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C20">
         <v>1370</v>
@@ -950,8 +1016,11 @@
       <c r="E20" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F20" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>23</v>
       </c>
@@ -967,8 +1036,11 @@
       <c r="E21" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F21" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
         <v>26</v>
       </c>
@@ -984,8 +1056,11 @@
       <c r="E22" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F22" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
         <v>27</v>
       </c>
@@ -1001,13 +1076,16 @@
       <c r="E23" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F23" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>28</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>48</v>
+        <v>67</v>
       </c>
       <c r="C24">
         <v>68531</v>
@@ -1018,13 +1096,16 @@
       <c r="E24" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F24" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C25">
         <v>21605</v>
@@ -1035,13 +1116,16 @@
       <c r="E25" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F25" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C26">
         <v>18540</v>
@@ -1052,13 +1136,16 @@
       <c r="E26" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F26" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>31</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C27">
         <v>81402</v>
@@ -1069,13 +1156,16 @@
       <c r="E27" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F27" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
         <v>44</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C28">
         <v>1478</v>
@@ -1086,19 +1176,22 @@
       <c r="E28" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F28" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="C29">
         <v>19509</v>
       </c>
       <c r="D29" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added info about channel type
</commit_message>
<xml_diff>
--- a/telegram_corpus.xlsx
+++ b/telegram_corpus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c315e0645f3ee56d/Data gov 50/Final project/gov50-final/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="263" documentId="8_{6E2AAD70-F8D2-44E6-9A27-31C793069EE0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D86A6682-A29A-4854-BB0E-440DDE9CA94E}"/>
+  <xr:revisionPtr revIDLastSave="337" documentId="8_{6E2AAD70-F8D2-44E6-9A27-31C793069EE0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{ED588D0D-AF37-4475-9313-10D81CE9FA41}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E642C494-3A5F-4C64-B3BD-CD15303C2502}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="77">
   <si>
     <t>Name</t>
   </si>
@@ -238,6 +238,33 @@
   </si>
   <si>
     <t>studentyBY</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Sources</t>
+  </si>
+  <si>
+    <t>Reporting</t>
+  </si>
+  <si>
+    <t>Reposting</t>
+  </si>
+  <si>
+    <t>Activist</t>
+  </si>
+  <si>
+    <t>Internal</t>
+  </si>
+  <si>
+    <t>Opinion</t>
+  </si>
+  <si>
+    <t>Crowdsourced</t>
+  </si>
+  <si>
+    <t>Other</t>
   </si>
 </sst>
 </file>
@@ -615,10 +642,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B79CD0CB-8193-4741-A468-87913EFFCABE}">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -626,9 +653,12 @@
     <col min="1" max="1" width="48.81640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.90625" customWidth="1"/>
     <col min="3" max="3" width="20.6328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -647,8 +677,14 @@
       <c r="F1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -667,8 +703,14 @@
       <c r="F2" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G2" t="s">
+        <v>72</v>
+      </c>
+      <c r="H2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -687,8 +729,14 @@
       <c r="F3" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G3" t="s">
+        <v>70</v>
+      </c>
+      <c r="H3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
@@ -707,8 +755,14 @@
       <c r="F4" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G4" t="s">
+        <v>72</v>
+      </c>
+      <c r="H4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
@@ -727,8 +781,14 @@
       <c r="F5" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G5" t="s">
+        <v>72</v>
+      </c>
+      <c r="H5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
@@ -747,8 +807,14 @@
       <c r="F6" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G6" t="s">
+        <v>72</v>
+      </c>
+      <c r="H6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
@@ -767,8 +833,14 @@
       <c r="F7" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G7" t="s">
+        <v>70</v>
+      </c>
+      <c r="H7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
@@ -787,8 +859,14 @@
       <c r="F8" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G8" t="s">
+        <v>70</v>
+      </c>
+      <c r="H8" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>8</v>
       </c>
@@ -807,8 +885,14 @@
       <c r="F9" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G9" t="s">
+        <v>70</v>
+      </c>
+      <c r="H9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>9</v>
       </c>
@@ -827,8 +911,14 @@
       <c r="F10" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G10" t="s">
+        <v>74</v>
+      </c>
+      <c r="H10" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -847,8 +937,14 @@
       <c r="F11" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G11" t="s">
+        <v>74</v>
+      </c>
+      <c r="H11" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -867,8 +963,14 @@
       <c r="F12" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G12" t="s">
+        <v>70</v>
+      </c>
+      <c r="H12" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>12</v>
       </c>
@@ -887,8 +989,14 @@
       <c r="F13" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G13" t="s">
+        <v>70</v>
+      </c>
+      <c r="H13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
         <v>13</v>
       </c>
@@ -907,8 +1015,14 @@
       <c r="F14" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G14" t="s">
+        <v>70</v>
+      </c>
+      <c r="H14" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -927,8 +1041,14 @@
       <c r="F15" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G15" t="s">
+        <v>72</v>
+      </c>
+      <c r="H15" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
         <v>15</v>
       </c>
@@ -940,7 +1060,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
@@ -959,8 +1079,14 @@
       <c r="F17" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G17" t="s">
+        <v>74</v>
+      </c>
+      <c r="H17" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>57</v>
       </c>
@@ -979,8 +1105,14 @@
       <c r="F18" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G18" t="s">
+        <v>76</v>
+      </c>
+      <c r="H18" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>58</v>
       </c>
@@ -999,8 +1131,14 @@
       <c r="F19" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G19" t="s">
+        <v>76</v>
+      </c>
+      <c r="H19" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>59</v>
       </c>
@@ -1019,8 +1157,14 @@
       <c r="F20" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G20" t="s">
+        <v>76</v>
+      </c>
+      <c r="H20" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>23</v>
       </c>
@@ -1039,8 +1183,14 @@
       <c r="F21" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G21" t="s">
+        <v>70</v>
+      </c>
+      <c r="H21" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
         <v>26</v>
       </c>
@@ -1059,8 +1209,14 @@
       <c r="F22" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G22" t="s">
+        <v>74</v>
+      </c>
+      <c r="H22" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
         <v>27</v>
       </c>
@@ -1079,8 +1235,14 @@
       <c r="F23" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G23" t="s">
+        <v>72</v>
+      </c>
+      <c r="H23" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>28</v>
       </c>
@@ -1099,8 +1261,14 @@
       <c r="F24" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G24" t="s">
+        <v>74</v>
+      </c>
+      <c r="H24" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
         <v>29</v>
       </c>
@@ -1119,8 +1287,14 @@
       <c r="F25" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G25" t="s">
+        <v>76</v>
+      </c>
+      <c r="H25" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
         <v>30</v>
       </c>
@@ -1139,8 +1313,14 @@
       <c r="F26" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G26" t="s">
+        <v>70</v>
+      </c>
+      <c r="H26" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>31</v>
       </c>
@@ -1159,8 +1339,14 @@
       <c r="F27" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G27" t="s">
+        <v>70</v>
+      </c>
+      <c r="H27" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
         <v>44</v>
       </c>
@@ -1179,8 +1365,14 @@
       <c r="F28" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G28" t="s">
+        <v>70</v>
+      </c>
+      <c r="H28" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" s="6" t="s">
         <v>52</v>
       </c>

</xml_diff>